<commit_message>
Added update and delete grade feature
</commit_message>
<xml_diff>
--- a/SGMS_Report.xlsx
+++ b/SGMS_Report.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,17 +434,60 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Assessment</t>
+          <t>Assessment Type</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Marks</t>
+          <t xml:space="preserve">Marks </t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Max Marks</t>
+          <t>Maximim Marks</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Date </t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Semester </t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>STU576</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Ssc</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>class assesment</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>100</v>
+      </c>
+      <c r="E2" t="n">
+        <v>200</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>07/08/2025</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>5th</t>
         </is>
       </c>
     </row>

</xml_diff>